<commit_message>
Aktualisierung cda-eav und Beispieldateien
</commit_message>
<xml_diff>
--- a/import-server/cda_basismodul/CDA Beispielpatienten.xlsx
+++ b/import-server/cda_basismodul/CDA Beispielpatienten.xlsx
@@ -781,13 +781,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CG7" sqref="CG7"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AI11" sqref="AI11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="87" max="87" width="23" bestFit="1" customWidth="1"/>
   </cols>
@@ -1148,9 +1151,7 @@
       <c r="AG2" s="2">
         <v>36.700000000000003</v>
       </c>
-      <c r="AH2" s="2">
-        <v>0</v>
-      </c>
+      <c r="AH2" s="2"/>
       <c r="AI2" s="2" t="s">
         <v>93</v>
       </c>
@@ -1368,9 +1369,7 @@
       <c r="AG3" s="2">
         <v>35.5</v>
       </c>
-      <c r="AH3" s="2">
-        <v>0</v>
-      </c>
+      <c r="AH3" s="2"/>
       <c r="AI3" s="2" t="s">
         <v>93</v>
       </c>
@@ -1586,9 +1585,7 @@
       <c r="AG4" s="2">
         <v>35.700000000000003</v>
       </c>
-      <c r="AH4" s="2">
-        <v>0</v>
-      </c>
+      <c r="AH4" s="2"/>
       <c r="AI4" s="2" t="s">
         <v>93</v>
       </c>

</xml_diff>